<commit_message>
fix(controllers): toposort supports drag & drop
</commit_message>
<xml_diff>
--- a/models/计算机_prerequisites.xlsx
+++ b/models/计算机_prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Files for Work\ds proj\courseSchedule\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C601AC-9013-4103-9260-EA6E95BE4B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886C1DE5-7DD1-446A-B3FD-1DA554F08FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1380" windowWidth="16956" windowHeight="10968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2124" yWindow="720" windowWidth="16956" windowHeight="10968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="206">
   <si>
     <t>courseID</t>
   </si>
@@ -678,10 +678,6 @@
   </si>
   <si>
     <t>0007366,0010663,0010719</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>9997366</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1063,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1585,7 @@
         <v>100</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1913,7 +1909,7 @@
         <v>160</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>